<commit_message>
add python and sql nav link
</commit_message>
<xml_diff>
--- a/documentation-and-dataset/full-stack-challenge.xlsx
+++ b/documentation-and-dataset/full-stack-challenge.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Full-Stack-Dev.-Challenge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Full-Stack-Dev.-Challenge\documentation-and-dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7932" windowHeight="8448" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7932" windowHeight="8448" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Foundations of JavaScript" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="API Security and Testing" sheetId="7" r:id="rId7"/>
     <sheet name="SSR &amp; Caching" sheetId="8" r:id="rId8"/>
     <sheet name="Real-time Comm &amp; WebSockets" sheetId="9" r:id="rId9"/>
+    <sheet name="SQL" sheetId="11" r:id="rId10"/>
+    <sheet name="Python" sheetId="12" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="FoundationsOfJavaScript">Table1[]</definedName>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="826">
   <si>
     <t>Challenge Number</t>
   </si>
@@ -3161,12 +3163,551 @@
 4. Price Statistics Computation (Web Worker): Compute the average, maximum, and minimum values of the "price" column.
 5. Results Transmission: Transmit the meticulously processed dataset, total revenue, and price statistics back to the main thread for further analysis or visualization.</t>
   </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>Subcategory</t>
+  </si>
+  <si>
+    <t>Foundation</t>
+  </si>
+  <si>
+    <t>SQL Basics</t>
+  </si>
+  <si>
+    <t>- Write a SQL query to retrieve the names and ages of all employees from the "employees" table. &lt;br&gt; - Create a new table named "customers" with columns for customer ID, name, and email address. &lt;br&gt; - Insert a new record into the "orders" table with the order ID, customer ID, and order date. &lt;br&gt; - Update the salary of an employee with ID 101 to $5000 in the "employees" table. &lt;br&gt; - Delete all records from the "products" table where the price is less than $10.</t>
+  </si>
+  <si>
+    <t>SQL Data Types</t>
+  </si>
+  <si>
+    <t>- Create a table named "students" with columns for student ID (integer), name (text), and age (integer). &lt;br&gt; - Insert records into the "students" table with various integer values for student ID and age. &lt;br&gt; - Calculate the average age of students in the "students" table. &lt;br&gt; - Update the age of a specific student in the "students" table. &lt;br&gt; - Delete records of students who are below 18 years old from the "students" table.</t>
+  </si>
+  <si>
+    <t>SQL Date Format</t>
+  </si>
+  <si>
+    <t>- Retrieve the current date in the format 'YYYY-MM-DD'. &lt;br&gt; - Convert a date string '2024-05-22' to the format 'DD/MM/YYYY'. &lt;br&gt; - Extract the year from a given date in the "orders" table. &lt;br&gt; - Calculate the difference in days between two dates. &lt;br&gt; - Retrieve records from the "sales" table where the sale date is between two specific dates.</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>Aggregate Functions</t>
+  </si>
+  <si>
+    <t>- Calculate the total sales amount for each product from the "sales" table. &lt;br&gt; - Determine the average rating of all products in the "ratings" table. &lt;br&gt; - Count the number of orders placed by each customer in the "orders" table. &lt;br&gt; - Find the maximum and minimum salaries of employees in the "employees" table. &lt;br&gt; - Calculate the total quantity of products sold in each category from the "sales" table.</t>
+  </si>
+  <si>
+    <t>Joins</t>
+  </si>
+  <si>
+    <t>- Retrieve the names of customers who placed orders along with their order IDs from the "customers" and "orders" tables. &lt;br&gt; - List all employees along with their department names from the "employees" and "departments" tables. &lt;br&gt; - Display product details along with their sales information from the "products" and "sales" tables. &lt;br&gt; - Show customer names, order IDs, and order dates along with product details from the "customers", "orders", and "products" tables. &lt;br&gt; - Retrieve employee names along with their manager names from the "employees" table using self-join.</t>
+  </si>
+  <si>
+    <t>Subqueries</t>
+  </si>
+  <si>
+    <t>- Find employees whose salary is higher than the average salary in the company from the "employees" table. &lt;br&gt; - List customers who have not placed any orders from the "customers" and "orders" tables using a subquery with NOT EXISTS. &lt;br&gt; - Display product details of the most expensive product from the "products" table using a subquery with the MAX function. &lt;br&gt; - Retrieve the names of employees who have sales records in the "sales" table using a correlated subquery. &lt;br&gt; - Calculate the total sales amount for each customer using a subquery in the SELECT statement.</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>Performance Tuning</t>
+  </si>
+  <si>
+    <t>- Identify and optimize slow-running queries in the database. &lt;br&gt; - Analyze and improve indexing strategies for frequently accessed tables. &lt;br&gt; - Implement caching mechanisms to reduce database load. &lt;br&gt; - Tune database configuration parameters for better performance. &lt;br&gt; - Monitor database performance metrics and optimize resource utilization.</t>
+  </si>
+  <si>
+    <t>Window Functions</t>
+  </si>
+  <si>
+    <t>- Calculate the cumulative sales amount for each month using a window function. &lt;br&gt; - Rank employees based on their sales performance using the RANK function. &lt;br&gt; - Determine the moving average of stock prices over a specific period using a window function. &lt;br&gt; - Calculate the running total of sales revenue for each product using the SUM function with the OVER clause. &lt;br&gt; - Identify outliers in a dataset using percentile calculations with window functions.</t>
+  </si>
+  <si>
+    <t>Pivoting Data</t>
+  </si>
+  <si>
+    <t>- Transform rows into columns to create a pivot table summarizing sales data by product category. &lt;br&gt; - Unpivot data from multiple columns into rows to normalize the dataset. &lt;br&gt; - Create dynamic pivot tables that automatically adjust to changes in data. &lt;br&gt; - Aggregate and pivot data to generate cross-tabulation reports for analysis. &lt;br&gt; - Compare sales performance across different regions using pivoted data.</t>
+  </si>
+  <si>
+    <t>Frameworks and Libraries</t>
+  </si>
+  <si>
+    <t>Oracle PL/SQL Programming</t>
+  </si>
+  <si>
+    <t>- Write a PL/SQL stored procedure to calculate employee bonuses based on performance ratings. &lt;br&gt; - Implement exception handling in PL/SQL code to handle errors gracefully. &lt;br&gt; - Create a PL/SQL function to validate user input and return the result. &lt;br&gt; - Use cursors in a PL/SQL program to iterate through query results and perform operations. &lt;br&gt; - Develop a trigger in PL/SQL to automatically update employee records when a new department is created.</t>
+  </si>
+  <si>
+    <t>SQL Cookbook</t>
+  </si>
+  <si>
+    <t>- Retrieve the top 10 highest-selling products from the "sales" table. &lt;br&gt; - Generate a report showing monthly sales trends for the past year. &lt;br&gt; - Calculate the total revenue generated by each product category. &lt;br&gt; - Find customers who have not made any purchases in the last three months. &lt;br&gt; - Implement pagination for displaying large result sets in web applications.</t>
+  </si>
+  <si>
+    <t>Tools and Techniques</t>
+  </si>
+  <si>
+    <t>SQL Practice Problems</t>
+  </si>
+  <si>
+    <t>- Solve a beginner-level SQL problem: Retrieve the names and ages of all students from the "students" table. &lt;br&gt; - Solve an intermediate-level SQL problem: Calculate the total sales amount for each product from the "sales" table. &lt;br&gt; - Solve an advanced-level SQL problem: Identify the top 5 customers with the highest total purchase amount. &lt;br&gt; - Solve a beginner-level SQL problem: Insert a new record into the "employees" table with employee ID, name, and salary. &lt;br&gt; - Solve an intermediate-level SQL problem: Retrieve the average rating of products in each category from the "products" and "ratings" tables.</t>
+  </si>
+  <si>
+    <t>SQL Beginner's Guide &amp; 7-Day Crash Course</t>
+  </si>
+  <si>
+    <t>- Complete Day 1: Getting Started - Set up PostgreSQL and execute your first SQL query. &lt;br&gt; - Complete Day 2: Basic Syntax - Learn about SELECT, FROM, WHERE clauses, and practice querying data. &lt;br&gt; - Complete Day 3: Practice Exercises - Solve beginner-level SQL exercises to reinforce your understanding. &lt;br&gt; - Complete Day 4: Intermediate Queries - Dive deeper into SQL with JOINS, GROUP BY, and aggregate functions. &lt;br&gt; - Complete Day 5: Advanced Techniques - Explore advanced SQL concepts like subqueries, window functions, and pivoting data.</t>
+  </si>
+  <si>
+    <t>Task Description</t>
+  </si>
+  <si>
+    <t>Fundamentals</t>
+  </si>
+  <si>
+    <t>Syntax</t>
+  </si>
+  <si>
+    <t>Write a Python script to print "Hello, World!" to the console.</t>
+  </si>
+  <si>
+    <t>Define variables for storing an integer, a float, and a string, and print their values.</t>
+  </si>
+  <si>
+    <t>Use Python's arithmetic operators to perform basic calculations and print the results.</t>
+  </si>
+  <si>
+    <t>Write a simple conditional statement to check if a given number is even or odd.</t>
+  </si>
+  <si>
+    <t>Define a list containing integers and print the elements using a loop.</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>Declare a variable to store your age and print a message using that variable.</t>
+  </si>
+  <si>
+    <t>Create variables to represent the length, width, and height of a box, and calculate its volume.</t>
+  </si>
+  <si>
+    <t>Define variables to store your name and favorite color, then print a message combining both.</t>
+  </si>
+  <si>
+    <t>Use variables to represent the price and quantity of a product, then calculate the total cost.</t>
+  </si>
+  <si>
+    <t>Assign a value to a variable and then reassign it to a different value, demonstrating variable mutation.</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>Create a list of your favorite foods and print each item on a separate line.</t>
+  </si>
+  <si>
+    <t>Define a tuple containing the names of the months of the year and print them.</t>
+  </si>
+  <si>
+    <t>Construct a dictionary representing a person's information (name, age, city), and print each key-value pair.</t>
+  </si>
+  <si>
+    <t>Access and print specific elements from a nested list or dictionary.</t>
+  </si>
+  <si>
+    <t>Use list comprehension to create a new list from an existing list with certain modifications.</t>
+  </si>
+  <si>
+    <t>Write a conditional statement to determine if a given year is a leap year.</t>
+  </si>
+  <si>
+    <t>Implement a voting eligibility check based on age using if-elif-else statements.</t>
+  </si>
+  <si>
+    <t>Create a program that categorizes a given number into positive, negative, or zero.</t>
+  </si>
+  <si>
+    <t>Use a nested if statement to determine a person's BMI category based on their height and weight.</t>
+  </si>
+  <si>
+    <t>Write a program to check if a given number is prime or composite using a loop and conditional statements.</t>
+  </si>
+  <si>
+    <t>Define a function to calculate the factorial of a given number and test it with different inputs.</t>
+  </si>
+  <si>
+    <t>Create a function to check if a given number is a prime number and use it to find all primes in a range.</t>
+  </si>
+  <si>
+    <t>Write a function to generate the Fibonacci sequence up to a specified limit and print the sequence.</t>
+  </si>
+  <si>
+    <t>Implement a function to calculate the area and perimeter of a rectangle given its length and width.</t>
+  </si>
+  <si>
+    <t>Define a function to calculate the square of a number and use it to create a list of squares.</t>
+  </si>
+  <si>
+    <t>File Handling</t>
+  </si>
+  <si>
+    <t>Read data from a text file, process it, and write the results to a new file.</t>
+  </si>
+  <si>
+    <t>Write a program to count the number of lines, words, and characters in a text file.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create a CSV file and write data to it using the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>csv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> module, then read and display the contents.</t>
+    </r>
+  </si>
+  <si>
+    <t>Use file handling to implement a simple text editor that allows users to write and save text files.</t>
+  </si>
+  <si>
+    <t>Write a program to search for a specific word in multiple text files and display the file names.</t>
+  </si>
+  <si>
+    <t>Implement error handling in a function that divides two numbers, handling ZeroDivisionError.</t>
+  </si>
+  <si>
+    <t>Write a program that reads user input for a number and handles ValueError if the input is not a number.</t>
+  </si>
+  <si>
+    <t>Create a function that opens a file and handles FileNotFoundError if the file does not exist.</t>
+  </si>
+  <si>
+    <t>Use try-except blocks to handle exceptions when accessing elements from a list or dictionary.</t>
+  </si>
+  <si>
+    <t>Write a program that reads data from a CSV file and handles exceptions that may occur during processing.</t>
+  </si>
+  <si>
+    <t>Modules</t>
+  </si>
+  <si>
+    <t>Create a custom module with functions for calculating area and perimeter of geometric shapes.</t>
+  </si>
+  <si>
+    <t>Define a module containing utility functions for common mathematical operations like factorial and square root.</t>
+  </si>
+  <si>
+    <t>Implement a module with functions for working with dates and times, such as calculating age and time differences.</t>
+  </si>
+  <si>
+    <t>Create a module that provides functions for generating random numbers and shuffling lists.</t>
+  </si>
+  <si>
+    <t>Define a module with functions for string manipulation, such as reversing a string and checking for palindromes.</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>Define a class representing a student with attributes like name, age, and methods for displaying information and updating attributes.</t>
+  </si>
+  <si>
+    <t>Create a class representing a bank account with methods for depositing, withdrawing, and checking the balance.</t>
+  </si>
+  <si>
+    <t>Implement a class representing a car with attributes like make, model, and methods for starting, stopping, and accelerating.</t>
+  </si>
+  <si>
+    <t>Define a class representing a book with attributes like title, author, and methods for borrowing and returning.</t>
+  </si>
+  <si>
+    <t>Create a class representing a restaurant with attributes like name, cuisine type, and methods for seating customers and taking orders.</t>
+  </si>
+  <si>
+    <t>Decorators</t>
+  </si>
+  <si>
+    <t>Implement a decorator function to log the execution time of another function.</t>
+  </si>
+  <si>
+    <t>Create a decorator that caches the results of a function to improve performance for repeated function calls.</t>
+  </si>
+  <si>
+    <t>Define a decorator to ensure that only authorized users have access to a specific function.</t>
+  </si>
+  <si>
+    <t>Write a decorator to validate the input arguments of a function before executing it.</t>
+  </si>
+  <si>
+    <t>Implement a decorator to retry a function call a specified number of times in case of failure.</t>
+  </si>
+  <si>
+    <t>Generators</t>
+  </si>
+  <si>
+    <t>Write a generator function to generate Fibonacci numbers up to a specified limit.</t>
+  </si>
+  <si>
+    <t>Implement a generator that yields prime numbers infinitely.</t>
+  </si>
+  <si>
+    <t>Create a generator to generate a sequence of random numbers within a specified range.</t>
+  </si>
+  <si>
+    <t>Define a generator function to generate permutations of a given list of elements.</t>
+  </si>
+  <si>
+    <t>Write a generator that generates all possible combinations of elements from a given list.</t>
+  </si>
+  <si>
+    <t>Context Managers</t>
+  </si>
+  <si>
+    <t>Create a context manager for opening and closing a file, ensuring proper resource management.</t>
+  </si>
+  <si>
+    <t>Implement a context manager for database transactions, ensuring that transactions are committed or rolled back properly.</t>
+  </si>
+  <si>
+    <t>Write a context manager for measuring the execution time of a block of code.</t>
+  </si>
+  <si>
+    <t>Define a context manager for acquiring and releasing locks to ensure thread safety.</t>
+  </si>
+  <si>
+    <t>Implement a context manager to handle connecting and disconnecting from a network socket.</t>
+  </si>
+  <si>
+    <t>Concurrency</t>
+  </si>
+  <si>
+    <t>Use threading to parallelize the execution of CPU-bound tasks, such as calculating Fibonacci numbers.</t>
+  </si>
+  <si>
+    <t>Implement multiprocessing to process multiple tasks concurrently, such as image processing.</t>
+  </si>
+  <si>
+    <t>Write a program using asyncio to perform asynchronous I/O operations, such as web scraping.</t>
+  </si>
+  <si>
+    <t>Use concurrent.futures module to execute tasks concurrently with ThreadPoolExecutor or ProcessPoolExecutor.</t>
+  </si>
+  <si>
+    <t>Create a producer-consumer application using threading or multiprocessing for task distribution.</t>
+  </si>
+  <si>
+    <t>Write a regular expression to validate email addresses and test it with different inputs.</t>
+  </si>
+  <si>
+    <t>Implement a regular expression to extract phone numbers from a given text.</t>
+  </si>
+  <si>
+    <t>Create a regex pattern to match URLs in a text and extract them.</t>
+  </si>
+  <si>
+    <t>Write a regex to find all occurrences of a specific word in a text document.</t>
+  </si>
+  <si>
+    <t>Use regular expressions to parse and extract data from a structured text format like CSV or JSON.</t>
+  </si>
+  <si>
+    <t>Libraries and Frameworks</t>
+  </si>
+  <si>
+    <t>NumPy</t>
+  </si>
+  <si>
+    <t>Use NumPy to perform basic array operations like creation, indexing, slicing, and mathematical computations.</t>
+  </si>
+  <si>
+    <t>Create a NumPy array from a Python list and perform element-wise mathematical operations on it.</t>
+  </si>
+  <si>
+    <t>Write a program to compute statistical measures such as mean, median, and standard deviation using NumPy.</t>
+  </si>
+  <si>
+    <t>Use NumPy to generate random numbers and perform operations like shuffling and sampling.</t>
+  </si>
+  <si>
+    <t>Implement broadcasting in NumPy to perform arithmetic operations on arrays with different shapes.</t>
+  </si>
+  <si>
+    <t>Pandas</t>
+  </si>
+  <si>
+    <t>Load a CSV file into a Pandas DataFrame, perform data exploration and manipulation operations (e.g., filtering, grouping, merging), and visualize the results with Matplotlib.</t>
+  </si>
+  <si>
+    <t>Use Pandas to handle missing data by filling, dropping, or interpolating missing values in a DataFrame.</t>
+  </si>
+  <si>
+    <t>Write a program to concatenate multiple DataFrames along rows and columns using Pandas.</t>
+  </si>
+  <si>
+    <t>Perform group-wise operations on a DataFrame using Pandas, such as groupby, aggregation, and transformation.</t>
+  </si>
+  <si>
+    <t>Utilize Pandas' powerful datetime functionality to work with date and time data in a DataFrame.</t>
+  </si>
+  <si>
+    <t>Create a simple Flask web application with routes for handling HTTP requests and rendering HTML templates.</t>
+  </si>
+  <si>
+    <t>Implement user authentication and authorization in a Flask application using Flask-Login and Flask-WTF.</t>
+  </si>
+  <si>
+    <t>Set up a RESTful API with Flask and implement CRUD operations (Create, Read, Update, Delete) for a resource.</t>
+  </si>
+  <si>
+    <t>Write unit tests for Flask routes and views using the Flask-Testing library.</t>
+  </si>
+  <si>
+    <t>Deploy a Flask application to a web server like Heroku or AWS Elastic Beanstalk.</t>
+  </si>
+  <si>
+    <t>Set up a Django project, define models for a basic database schema, create views and templates for a web application, and run the development server.</t>
+  </si>
+  <si>
+    <t>Implement user registration and login functionality in a Django application using Django's built-in authentication system.</t>
+  </si>
+  <si>
+    <t>Create an admin interface for managing application data using Django's admin site.</t>
+  </si>
+  <si>
+    <t>Develop a RESTful API with Django Rest Framework (DRF) for serving JSON data to client-side applications.</t>
+  </si>
+  <si>
+    <t>Use Django's middleware framework to add custom functionality to request/response processing.</t>
+  </si>
+  <si>
+    <t>TensorFlow</t>
+  </si>
+  <si>
+    <t>Build and train a simple neural network model using TensorFlow for a classification task (e.g., image recognition).</t>
+  </si>
+  <si>
+    <t>Implement transfer learning with TensorFlow by fine-tuning a pre-trained deep learning model.</t>
+  </si>
+  <si>
+    <t>Write a TensorFlow program to perform text classification using recurrent neural networks (RNNs).</t>
+  </si>
+  <si>
+    <t>Use TensorFlow to develop a recommendation system based on collaborative filtering techniques.</t>
+  </si>
+  <si>
+    <t>Deploy a TensorFlow model to production using TensorFlow Serving or TensorFlow Lite for mobile applications.</t>
+  </si>
+  <si>
+    <t>Solve a beginner-level SQL problem: Retrieve the names and ages of all students from the "students" table.</t>
+  </si>
+  <si>
+    <t>Solve an intermediate-level SQL problem: Calculate the total sales amount for each product from the "sales" table.</t>
+  </si>
+  <si>
+    <t>Solve an advanced-level SQL problem: Identify the top 5 customers with the highest total purchase amount.</t>
+  </si>
+  <si>
+    <t>Solve a beginner-level SQL problem: Insert a new record into the "employees" table with employee ID, name, and salary.</t>
+  </si>
+  <si>
+    <t>Solve an intermediate-level SQL problem: Retrieve the average rating of products in each category from the "products" and "ratings" tables.</t>
+  </si>
+  <si>
+    <t>Complete Day 1: Getting Started - Set up PostgreSQL and execute your first SQL query.</t>
+  </si>
+  <si>
+    <t>Complete Day 2: Basic Syntax - Learn about SELECT, FROM, WHERE clauses, and practice querying data.</t>
+  </si>
+  <si>
+    <t>Complete Day 3: Practice Exercises - Solve beginner-level SQL exercises to reinforce your understanding.</t>
+  </si>
+  <si>
+    <t>Complete Day 4: Intermediate Queries - Dive deeper into SQL with JOINS, GROUP BY, and aggregate functions.</t>
+  </si>
+  <si>
+    <t>Complete Day 5: Advanced Techniques - Explore advanced SQL concepts like subqueries, window functions, and pivoting data.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3218,6 +3759,18 @@
     </font>
     <font>
       <sz val="8"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
       <color rgb="FF0D0D0D"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -3358,7 +3911,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3489,6 +4042,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4854,8 +5416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="A97" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4882,8 +5444,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="14">
-        <v>1</v>
+      <c r="A2" s="15" t="s">
+        <v>653</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>3</v>
@@ -4934,8 +5496,8 @@
       <c r="D7" s="14"/>
     </row>
     <row r="8" spans="1:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="A8" s="14">
-        <v>2</v>
+      <c r="A8" s="15" t="s">
+        <v>654</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>5</v>
@@ -4986,8 +5548,8 @@
       <c r="D13" s="11"/>
     </row>
     <row r="14" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="11">
-        <v>3</v>
+      <c r="A14" s="13" t="s">
+        <v>655</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>7</v>
@@ -5038,8 +5600,8 @@
       <c r="D19" s="12"/>
     </row>
     <row r="20" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="11">
-        <v>4</v>
+      <c r="A20" s="13" t="s">
+        <v>656</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>9</v>
@@ -5090,8 +5652,8 @@
       <c r="D25" s="12"/>
     </row>
     <row r="26" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="11">
-        <v>5</v>
+      <c r="A26" s="13" t="s">
+        <v>657</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>11</v>
@@ -5142,8 +5704,8 @@
       <c r="D31" s="12"/>
     </row>
     <row r="32" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="11">
-        <v>6</v>
+      <c r="A32" s="13" t="s">
+        <v>658</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>13</v>
@@ -5194,8 +5756,8 @@
       <c r="D37" s="13"/>
     </row>
     <row r="38" spans="1:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="A38" s="11">
-        <v>7</v>
+      <c r="A38" s="13" t="s">
+        <v>659</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>15</v>
@@ -5246,10 +5808,10 @@
       <c r="D43" s="13"/>
     </row>
     <row r="44" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="11">
-        <v>8</v>
-      </c>
-      <c r="B44" s="11" t="s">
+      <c r="A44" s="13" t="s">
+        <v>660</v>
+      </c>
+      <c r="B44" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C44" s="11" t="s">
@@ -5298,10 +5860,10 @@
       <c r="D49" s="13"/>
     </row>
     <row r="50" spans="1:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="A50" s="11">
-        <v>9</v>
-      </c>
-      <c r="B50" s="11" t="s">
+      <c r="A50" s="13" t="s">
+        <v>661</v>
+      </c>
+      <c r="B50" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C50" s="13" t="s">
@@ -5350,10 +5912,10 @@
       <c r="D55" s="13"/>
     </row>
     <row r="56" spans="1:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="A56" s="11">
-        <v>10</v>
-      </c>
-      <c r="B56" s="11" t="s">
+      <c r="A56" s="13" t="s">
+        <v>662</v>
+      </c>
+      <c r="B56" s="13" t="s">
         <v>21</v>
       </c>
       <c r="C56" s="11" t="s">
@@ -5410,10 +5972,10 @@
       <c r="D62" s="13"/>
     </row>
     <row r="63" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="11">
-        <v>11</v>
-      </c>
-      <c r="B63" s="11" t="s">
+      <c r="A63" s="13" t="s">
+        <v>663</v>
+      </c>
+      <c r="B63" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C63" s="11" t="s">
@@ -5470,10 +6032,10 @@
       <c r="D69" s="13"/>
     </row>
     <row r="70" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A70" s="11">
-        <v>12</v>
-      </c>
-      <c r="B70" s="11" t="s">
+      <c r="A70" s="13" t="s">
+        <v>664</v>
+      </c>
+      <c r="B70" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C70" s="11" t="s">
@@ -5522,10 +6084,10 @@
       <c r="D75" s="13"/>
     </row>
     <row r="76" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="11">
-        <v>13</v>
-      </c>
-      <c r="B76" s="11" t="s">
+      <c r="A76" s="13" t="s">
+        <v>665</v>
+      </c>
+      <c r="B76" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C76" s="11" t="s">
@@ -5574,8 +6136,8 @@
       <c r="D81" s="13"/>
     </row>
     <row r="82" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="11">
-        <v>14</v>
+      <c r="A82" s="13" t="s">
+        <v>666</v>
       </c>
       <c r="B82" s="11" t="s">
         <v>29</v>
@@ -5626,8 +6188,8 @@
       <c r="D87" s="13"/>
     </row>
     <row r="88" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="11">
-        <v>15</v>
+      <c r="A88" s="13" t="s">
+        <v>667</v>
       </c>
       <c r="B88" s="11" t="s">
         <v>11</v>
@@ -5678,8 +6240,8 @@
       <c r="D93" s="13"/>
     </row>
     <row r="94" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A94" s="11">
-        <v>16</v>
+      <c r="A94" s="13" t="s">
+        <v>668</v>
       </c>
       <c r="B94" s="11" t="s">
         <v>32</v>
@@ -5730,8 +6292,8 @@
       <c r="D99" s="13"/>
     </row>
     <row r="100" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="11">
-        <v>17</v>
+      <c r="A100" s="13" t="s">
+        <v>669</v>
       </c>
       <c r="B100" s="11" t="s">
         <v>34</v>
@@ -5782,8 +6344,8 @@
       <c r="D105" s="13"/>
     </row>
     <row r="106" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A106" s="11">
-        <v>18</v>
+      <c r="A106" s="13" t="s">
+        <v>670</v>
       </c>
       <c r="B106" s="11" t="s">
         <v>36</v>
@@ -5834,8 +6396,8 @@
       <c r="D111" s="13"/>
     </row>
     <row r="112" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="11">
-        <v>19</v>
+      <c r="A112" s="13" t="s">
+        <v>671</v>
       </c>
       <c r="B112" s="11" t="s">
         <v>38</v>
@@ -5886,8 +6448,8 @@
       <c r="D117" s="13"/>
     </row>
     <row r="118" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A118" s="11">
-        <v>20</v>
+      <c r="A118" s="13" t="s">
+        <v>672</v>
       </c>
       <c r="B118" s="11" t="s">
         <v>40</v>
@@ -5940,12 +6502,1260 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>673</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>398</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>673</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>398</v>
+      </c>
+      <c r="I1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="47" t="s">
+        <v>673</v>
+      </c>
+      <c r="K1" s="48" t="s">
+        <v>398</v>
+      </c>
+      <c r="M1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="47" t="s">
+        <v>673</v>
+      </c>
+      <c r="O1" s="48" t="s">
+        <v>398</v>
+      </c>
+      <c r="Q1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="47" t="s">
+        <v>673</v>
+      </c>
+      <c r="S1" s="48" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="49" t="s">
+        <v>674</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>675</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>676</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F2" s="49" t="s">
+        <v>682</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>683</v>
+      </c>
+      <c r="I2" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J2" s="49" t="s">
+        <v>689</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>690</v>
+      </c>
+      <c r="M2" s="49" t="s">
+        <v>695</v>
+      </c>
+      <c r="N2" s="49" t="s">
+        <v>696</v>
+      </c>
+      <c r="O2" s="41" t="s">
+        <v>697</v>
+      </c>
+      <c r="Q2" s="49" t="s">
+        <v>700</v>
+      </c>
+      <c r="R2" s="49" t="s">
+        <v>701</v>
+      </c>
+      <c r="S2" s="41" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="49" t="s">
+        <v>674</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>677</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>678</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F3" s="49" t="s">
+        <v>684</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>685</v>
+      </c>
+      <c r="I3" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J3" s="49" t="s">
+        <v>691</v>
+      </c>
+      <c r="K3" s="41" t="s">
+        <v>692</v>
+      </c>
+      <c r="M3" s="49" t="s">
+        <v>695</v>
+      </c>
+      <c r="N3" s="49" t="s">
+        <v>698</v>
+      </c>
+      <c r="O3" s="41" t="s">
+        <v>699</v>
+      </c>
+      <c r="Q3" s="49" t="s">
+        <v>700</v>
+      </c>
+      <c r="R3" s="49" t="s">
+        <v>703</v>
+      </c>
+      <c r="S3" s="41" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="49" t="s">
+        <v>674</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>679</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>680</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F4" s="49" t="s">
+        <v>686</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>687</v>
+      </c>
+      <c r="I4" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J4" s="49" t="s">
+        <v>693</v>
+      </c>
+      <c r="K4" s="41" t="s">
+        <v>694</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7:S11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:19" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>673</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>705</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>673</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>705</v>
+      </c>
+      <c r="I1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="47" t="s">
+        <v>673</v>
+      </c>
+      <c r="K1" s="48" t="s">
+        <v>705</v>
+      </c>
+      <c r="M1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="47" t="s">
+        <v>673</v>
+      </c>
+      <c r="O1" s="48" t="s">
+        <v>705</v>
+      </c>
+      <c r="Q1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="47" t="s">
+        <v>673</v>
+      </c>
+      <c r="S1" s="48" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="207.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>707</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>708</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F2" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>730</v>
+      </c>
+      <c r="I2" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J2" s="49" t="s">
+        <v>758</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>759</v>
+      </c>
+      <c r="M2" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N2" s="49" t="s">
+        <v>788</v>
+      </c>
+      <c r="O2" s="41" t="s">
+        <v>789</v>
+      </c>
+      <c r="Q2" s="49" t="s">
+        <v>700</v>
+      </c>
+      <c r="R2" s="49" t="s">
+        <v>701</v>
+      </c>
+      <c r="S2" s="41" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>707</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>709</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F3" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>731</v>
+      </c>
+      <c r="I3" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J3" s="49" t="s">
+        <v>758</v>
+      </c>
+      <c r="K3" s="41" t="s">
+        <v>760</v>
+      </c>
+      <c r="M3" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N3" s="49" t="s">
+        <v>788</v>
+      </c>
+      <c r="O3" s="41" t="s">
+        <v>790</v>
+      </c>
+      <c r="Q3" s="49" t="s">
+        <v>700</v>
+      </c>
+      <c r="R3" s="49" t="s">
+        <v>701</v>
+      </c>
+      <c r="S3" s="41" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>707</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>710</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F4" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>732</v>
+      </c>
+      <c r="I4" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J4" s="49" t="s">
+        <v>758</v>
+      </c>
+      <c r="K4" s="41" t="s">
+        <v>761</v>
+      </c>
+      <c r="M4" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N4" s="49" t="s">
+        <v>788</v>
+      </c>
+      <c r="O4" s="41" t="s">
+        <v>791</v>
+      </c>
+      <c r="Q4" s="49" t="s">
+        <v>700</v>
+      </c>
+      <c r="R4" s="49" t="s">
+        <v>701</v>
+      </c>
+      <c r="S4" s="41" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="207.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>707</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>711</v>
+      </c>
+      <c r="E5" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F5" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>733</v>
+      </c>
+      <c r="I5" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J5" s="49" t="s">
+        <v>758</v>
+      </c>
+      <c r="K5" s="41" t="s">
+        <v>762</v>
+      </c>
+      <c r="M5" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N5" s="49" t="s">
+        <v>788</v>
+      </c>
+      <c r="O5" s="41" t="s">
+        <v>792</v>
+      </c>
+      <c r="Q5" s="49" t="s">
+        <v>700</v>
+      </c>
+      <c r="R5" s="49" t="s">
+        <v>701</v>
+      </c>
+      <c r="S5" s="41" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="235.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>707</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>712</v>
+      </c>
+      <c r="E6" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F6" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>734</v>
+      </c>
+      <c r="I6" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J6" s="49" t="s">
+        <v>758</v>
+      </c>
+      <c r="K6" s="41" t="s">
+        <v>763</v>
+      </c>
+      <c r="M6" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N6" s="49" t="s">
+        <v>788</v>
+      </c>
+      <c r="O6" s="41" t="s">
+        <v>793</v>
+      </c>
+      <c r="Q6" s="49" t="s">
+        <v>700</v>
+      </c>
+      <c r="R6" s="49" t="s">
+        <v>701</v>
+      </c>
+      <c r="S6" s="41" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="331.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>713</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>714</v>
+      </c>
+      <c r="E7" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F7" s="49" t="s">
+        <v>735</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>736</v>
+      </c>
+      <c r="I7" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J7" s="49" t="s">
+        <v>764</v>
+      </c>
+      <c r="K7" s="41" t="s">
+        <v>765</v>
+      </c>
+      <c r="M7" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N7" s="49" t="s">
+        <v>794</v>
+      </c>
+      <c r="O7" s="41" t="s">
+        <v>795</v>
+      </c>
+      <c r="Q7" s="49" t="s">
+        <v>700</v>
+      </c>
+      <c r="R7" s="49" t="s">
+        <v>703</v>
+      </c>
+      <c r="S7" s="41" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="207.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>713</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>715</v>
+      </c>
+      <c r="E8" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F8" s="49" t="s">
+        <v>735</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>737</v>
+      </c>
+      <c r="I8" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J8" s="49" t="s">
+        <v>764</v>
+      </c>
+      <c r="K8" s="41" t="s">
+        <v>766</v>
+      </c>
+      <c r="M8" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N8" s="49" t="s">
+        <v>794</v>
+      </c>
+      <c r="O8" s="41" t="s">
+        <v>796</v>
+      </c>
+      <c r="Q8" s="49" t="s">
+        <v>700</v>
+      </c>
+      <c r="R8" s="49" t="s">
+        <v>703</v>
+      </c>
+      <c r="S8" s="41" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="180" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>713</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>716</v>
+      </c>
+      <c r="E9" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F9" s="49" t="s">
+        <v>735</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>738</v>
+      </c>
+      <c r="I9" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J9" s="49" t="s">
+        <v>764</v>
+      </c>
+      <c r="K9" s="41" t="s">
+        <v>767</v>
+      </c>
+      <c r="M9" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N9" s="49" t="s">
+        <v>794</v>
+      </c>
+      <c r="O9" s="41" t="s">
+        <v>797</v>
+      </c>
+      <c r="Q9" s="49" t="s">
+        <v>700</v>
+      </c>
+      <c r="R9" s="49" t="s">
+        <v>703</v>
+      </c>
+      <c r="S9" s="41" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>713</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>717</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F10" s="49" t="s">
+        <v>735</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>739</v>
+      </c>
+      <c r="I10" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J10" s="49" t="s">
+        <v>764</v>
+      </c>
+      <c r="K10" s="41" t="s">
+        <v>768</v>
+      </c>
+      <c r="M10" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N10" s="49" t="s">
+        <v>794</v>
+      </c>
+      <c r="O10" s="41" t="s">
+        <v>798</v>
+      </c>
+      <c r="Q10" s="49" t="s">
+        <v>700</v>
+      </c>
+      <c r="R10" s="49" t="s">
+        <v>703</v>
+      </c>
+      <c r="S10" s="41" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="221.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>713</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>718</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F11" s="49" t="s">
+        <v>735</v>
+      </c>
+      <c r="G11" s="41" t="s">
+        <v>740</v>
+      </c>
+      <c r="I11" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J11" s="49" t="s">
+        <v>764</v>
+      </c>
+      <c r="K11" s="41" t="s">
+        <v>769</v>
+      </c>
+      <c r="M11" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N11" s="49" t="s">
+        <v>794</v>
+      </c>
+      <c r="O11" s="41" t="s">
+        <v>799</v>
+      </c>
+      <c r="Q11" s="49" t="s">
+        <v>700</v>
+      </c>
+      <c r="R11" s="49" t="s">
+        <v>703</v>
+      </c>
+      <c r="S11" s="41" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="180" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>719</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>720</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F12" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>741</v>
+      </c>
+      <c r="I12" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J12" s="49" t="s">
+        <v>770</v>
+      </c>
+      <c r="K12" s="41" t="s">
+        <v>771</v>
+      </c>
+      <c r="M12" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N12" s="49" t="s">
+        <v>243</v>
+      </c>
+      <c r="O12" s="41" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="221.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>719</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>721</v>
+      </c>
+      <c r="E13" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F13" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>742</v>
+      </c>
+      <c r="I13" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J13" s="49" t="s">
+        <v>770</v>
+      </c>
+      <c r="K13" s="41" t="s">
+        <v>772</v>
+      </c>
+      <c r="M13" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N13" s="49" t="s">
+        <v>243</v>
+      </c>
+      <c r="O13" s="41" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="180" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>719</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>722</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F14" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>743</v>
+      </c>
+      <c r="I14" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J14" s="49" t="s">
+        <v>770</v>
+      </c>
+      <c r="K14" s="41" t="s">
+        <v>773</v>
+      </c>
+      <c r="M14" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N14" s="49" t="s">
+        <v>243</v>
+      </c>
+      <c r="O14" s="41" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="166.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>719</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>723</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F15" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>744</v>
+      </c>
+      <c r="I15" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J15" s="49" t="s">
+        <v>770</v>
+      </c>
+      <c r="K15" s="41" t="s">
+        <v>774</v>
+      </c>
+      <c r="M15" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N15" s="49" t="s">
+        <v>243</v>
+      </c>
+      <c r="O15" s="41" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>719</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>724</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F16" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>745</v>
+      </c>
+      <c r="I16" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J16" s="49" t="s">
+        <v>770</v>
+      </c>
+      <c r="K16" s="41" t="s">
+        <v>775</v>
+      </c>
+      <c r="M16" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N16" s="49" t="s">
+        <v>243</v>
+      </c>
+      <c r="O16" s="41" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="249" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B17" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>725</v>
+      </c>
+      <c r="E17" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F17" s="49" t="s">
+        <v>746</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>747</v>
+      </c>
+      <c r="I17" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J17" s="49" t="s">
+        <v>776</v>
+      </c>
+      <c r="K17" s="41" t="s">
+        <v>777</v>
+      </c>
+      <c r="M17" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N17" s="49" t="s">
+        <v>241</v>
+      </c>
+      <c r="O17" s="41" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="207.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B18" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>726</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F18" s="49" t="s">
+        <v>746</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>748</v>
+      </c>
+      <c r="I18" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J18" s="49" t="s">
+        <v>776</v>
+      </c>
+      <c r="K18" s="41" t="s">
+        <v>778</v>
+      </c>
+      <c r="M18" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N18" s="49" t="s">
+        <v>241</v>
+      </c>
+      <c r="O18" s="41" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="207.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>727</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F19" s="49" t="s">
+        <v>746</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>749</v>
+      </c>
+      <c r="I19" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J19" s="49" t="s">
+        <v>776</v>
+      </c>
+      <c r="K19" s="41" t="s">
+        <v>779</v>
+      </c>
+      <c r="M19" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N19" s="49" t="s">
+        <v>241</v>
+      </c>
+      <c r="O19" s="41" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>728</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F20" s="49" t="s">
+        <v>746</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>750</v>
+      </c>
+      <c r="I20" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J20" s="49" t="s">
+        <v>776</v>
+      </c>
+      <c r="K20" s="41" t="s">
+        <v>780</v>
+      </c>
+      <c r="M20" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N20" s="49" t="s">
+        <v>241</v>
+      </c>
+      <c r="O20" s="41" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="207.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="49" t="s">
+        <v>706</v>
+      </c>
+      <c r="B21" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>729</v>
+      </c>
+      <c r="E21" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F21" s="49" t="s">
+        <v>746</v>
+      </c>
+      <c r="G21" s="41" t="s">
+        <v>751</v>
+      </c>
+      <c r="I21" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J21" s="49" t="s">
+        <v>776</v>
+      </c>
+      <c r="K21" s="41" t="s">
+        <v>781</v>
+      </c>
+      <c r="M21" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N21" s="49" t="s">
+        <v>241</v>
+      </c>
+      <c r="O21" s="41" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="221.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F22" s="49" t="s">
+        <v>752</v>
+      </c>
+      <c r="G22" s="41" t="s">
+        <v>753</v>
+      </c>
+      <c r="I22" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J22" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="41" t="s">
+        <v>782</v>
+      </c>
+      <c r="M22" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N22" s="49" t="s">
+        <v>810</v>
+      </c>
+      <c r="O22" s="41" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="207.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F23" s="49" t="s">
+        <v>752</v>
+      </c>
+      <c r="G23" s="41" t="s">
+        <v>754</v>
+      </c>
+      <c r="I23" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J23" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="41" t="s">
+        <v>783</v>
+      </c>
+      <c r="M23" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N23" s="49" t="s">
+        <v>810</v>
+      </c>
+      <c r="O23" s="41" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="221.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E24" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F24" s="49" t="s">
+        <v>752</v>
+      </c>
+      <c r="G24" s="41" t="s">
+        <v>755</v>
+      </c>
+      <c r="I24" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J24" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="41" t="s">
+        <v>784</v>
+      </c>
+      <c r="M24" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N24" s="49" t="s">
+        <v>810</v>
+      </c>
+      <c r="O24" s="41" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F25" s="49" t="s">
+        <v>752</v>
+      </c>
+      <c r="G25" s="41" t="s">
+        <v>756</v>
+      </c>
+      <c r="I25" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J25" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="41" t="s">
+        <v>785</v>
+      </c>
+      <c r="M25" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N25" s="49" t="s">
+        <v>810</v>
+      </c>
+      <c r="O25" s="41" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="235.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="49" t="s">
+        <v>681</v>
+      </c>
+      <c r="F26" s="49" t="s">
+        <v>752</v>
+      </c>
+      <c r="G26" s="41" t="s">
+        <v>757</v>
+      </c>
+      <c r="I26" s="49" t="s">
+        <v>688</v>
+      </c>
+      <c r="J26" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="41" t="s">
+        <v>786</v>
+      </c>
+      <c r="M26" s="49" t="s">
+        <v>787</v>
+      </c>
+      <c r="N26" s="49" t="s">
+        <v>810</v>
+      </c>
+      <c r="O26" s="41" t="s">
+        <v>815</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F120"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A54" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7019,8 +8829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="B3" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7694,7 +9504,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="138.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="124.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="25">
         <v>77</v>
       </c>
@@ -8191,7 +10001,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="235.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="180" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>3</v>
       </c>

</xml_diff>